<commit_message>
sucessfull scope test of led driver timing
</commit_message>
<xml_diff>
--- a/dwg/LedDriverTiming.xlsx
+++ b/dwg/LedDriverTiming.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>f</t>
   </si>
@@ -117,6 +118,45 @@
   </si>
   <si>
     <t>reset time</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>G7</t>
+  </si>
+  <si>
+    <t>G6</t>
+  </si>
+  <si>
+    <t>G5</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>G3</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G0</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
+    <t>0x11011011</t>
   </si>
 </sst>
 </file>
@@ -144,18 +184,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -173,7 +207,6 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -181,11 +214,73 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -495,55 +590,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1">
+        <f>2.6*10^6</f>
+        <v>2600000</v>
+      </c>
+      <c r="C1" s="1">
         <f>2.7*10^6</f>
         <v>2700000</v>
       </c>
+      <c r="D1" s="1">
+        <f>2.4*10^6</f>
+        <v>2400000</v>
+      </c>
       <c r="H1" t="s">
         <v>25</v>
       </c>
       <c r="I1" s="1">
         <f>9.5*B2</f>
-        <v>3.5185185185185183E-6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3.6538461538461538E-6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <f>1/B1</f>
-        <v>3.7037037037037036E-7</v>
+        <v>3.8461538461538463E-7</v>
       </c>
       <c r="H2" t="s">
         <v>27</v>
       </c>
       <c r="I2" s="1">
         <f>I1/3</f>
-        <v>1.1728395061728394E-6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1.217948717948718E-6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -556,10 +658,10 @@
       </c>
       <c r="I3" s="1">
         <f>I2*24</f>
-        <v>2.8148148148148143E-5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2.9230769230769234E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -572,19 +674,19 @@
       </c>
       <c r="I4" s="1">
         <f>I3*100+B4</f>
-        <v>2.8648148148148144E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2.9730769230769233E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H5" t="s">
         <v>29</v>
       </c>
       <c r="I5" s="1">
         <f>1/I4</f>
-        <v>349.06270200387854</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>336.35187580853813</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -601,7 +703,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -619,10 +721,14 @@
       </c>
       <c r="E7" s="1">
         <f>1*$B$2</f>
-        <v>3.7037037037037036E-7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3.8461538461538463E-7</v>
+      </c>
+      <c r="G7" s="1">
+        <f>E7-C7</f>
+        <v>1.8461538461538466E-7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -640,10 +746,14 @@
       </c>
       <c r="E8" s="1">
         <f>2*$B$2</f>
-        <v>7.4074074074074073E-7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>7.6923076923076925E-7</v>
+      </c>
+      <c r="G8" s="1">
+        <f>E8-C8</f>
+        <v>2.1923076923076933E-7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -661,10 +771,23 @@
       </c>
       <c r="E9" s="1">
         <f>2*$B$2</f>
-        <v>7.4074074074074073E-7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>7.6923076923076925E-7</v>
+      </c>
+      <c r="G9" s="1">
+        <f>E9-C9</f>
+        <v>1.1923076923076934E-7</v>
+      </c>
+      <c r="H9">
+        <v>2.7</v>
+      </c>
+      <c r="I9">
+        <v>2.65</v>
+      </c>
+      <c r="J9">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -680,17 +803,23 @@
         <f t="shared" si="1"/>
         <v>7.5000000000000002E-7</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="9">
         <f>1*$B$2</f>
-        <v>3.7037037037037036E-7</v>
+        <v>3.8461538461538463E-7</v>
       </c>
       <c r="G10" s="1">
         <f>E10-C10</f>
+        <v>-6.53846153846153E-8</v>
+      </c>
+      <c r="H10" s="1">
         <v>-7.9629629629629563E-8</v>
       </c>
-      <c r="H10" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="1">
+        <v>-7.2641509433962205E-8</v>
+      </c>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -708,10 +837,15 @@
       </c>
       <c r="E12" s="1">
         <f>2.5*$B$2</f>
-        <v>9.2592592592592594E-7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>9.6153846153846149E-7</v>
+      </c>
+      <c r="G12" s="1">
+        <f>E12-C12</f>
+        <v>3.1153846153846157E-7</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -729,7 +863,11 @@
       </c>
       <c r="E13" s="1">
         <f>1.5*$B$2</f>
-        <v>5.5555555555555552E-7</v>
+        <v>5.7692307692307691E-7</v>
+      </c>
+      <c r="G13" s="1">
+        <f>E13-C13</f>
+        <v>1.2692307692307699E-7</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -738,25 +876,25 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="7">
         <v>0</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="7">
         <v>16</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -770,15 +908,15 @@
         <f>460.8*10^3</f>
         <v>460800</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <f>2*10^6</f>
         <v>2000000</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="8">
         <f>2.7*10^6</f>
         <v>2700000</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="8">
         <f>3*10^6</f>
         <v>3000000</v>
       </c>
@@ -791,19 +929,19 @@
         <f>B23/B27/$B19</f>
         <v>1199.9400029998501</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="8">
         <f>C23/C27/$B19</f>
         <v>470588.23529411765</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D21" s="8">
         <f>D23/D27/$B19</f>
         <v>2000000</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="8">
         <f>E23/E27/$B19</f>
         <v>2666666.6666666665</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="8">
         <f>F23/F27/$B19</f>
         <v>3000000</v>
       </c>
@@ -812,23 +950,23 @@
       <c r="A22" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <f>(B21-B20)/B20</f>
         <v>-4.9997500124921622E-5</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2">
         <f>(C21-C20)/C20</f>
         <v>2.1241830065359485E-2</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2">
         <f>(D21-D20)/D20</f>
         <v>0</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <f>(E21-E20)/E20</f>
         <v>-1.2345679012345737E-2</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="2">
         <f>(F21-F20)/F20</f>
         <v>0</v>
       </c>
@@ -862,23 +1000,23 @@
       <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <f>B23/B20/$B19</f>
         <v>416.66666666666669</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5">
         <f>C23/C20/$B19</f>
         <v>1.0850694444444444</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <f>D23/D20/$B19</f>
         <v>0.75</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="5">
         <f>E23/E20/$B19</f>
         <v>0.55555555555555558</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="5">
         <f>F23/F20/$B19</f>
         <v>0.5</v>
       </c>
@@ -887,23 +1025,23 @@
       <c r="A25" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="3">
         <f>FLOOR(B24,1)</f>
         <v>416</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="3">
         <f>FLOOR(C24,1)</f>
         <v>1</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="3">
         <f>FLOOR(D24,1)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="3">
         <f>FLOOR(E24,1)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F25" s="3">
         <f>FLOOR(F24,1)</f>
         <v>0</v>
       </c>
@@ -912,23 +1050,23 @@
       <c r="A26" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="3">
         <f>ROUND((B24-B25)*$B19,0)</f>
         <v>11</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="3">
         <f>ROUND((C24-C25)*$B19,0)</f>
         <v>1</v>
       </c>
-      <c r="D26" s="4">
+      <c r="D26" s="3">
         <f>ROUND((D24-D25)*$B19,0)</f>
         <v>12</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="3">
         <f>ROUND((E24-E25)*$B19,0)</f>
         <v>9</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F26" s="3">
         <f>ROUND((F24-F25)*$B19,0)</f>
         <v>8</v>
       </c>
@@ -937,46 +1075,46 @@
       <c r="A27" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="5">
         <f>B25+B26/$B19</f>
         <v>416.6875</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="5">
         <f>C25+C26/$B19</f>
         <v>1.0625</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <f>D25+D26/$B19</f>
         <v>0.75</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="5">
         <f>E25+E26/$B19</f>
         <v>0.5625</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="5">
         <f>F25+F26/$B19</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30" s="7">
         <v>1</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="C30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31" s="7">
         <v>8</v>
       </c>
-      <c r="C31" s="5"/>
+      <c r="C31" s="4"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -986,19 +1124,19 @@
         <f>1.2*10^3</f>
         <v>1200</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="8">
         <f>460.8*10^3</f>
         <v>460800</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="8">
         <f>2*10^6</f>
         <v>2000000</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="8">
         <f>2.7*10^6</f>
         <v>2700000</v>
       </c>
-      <c r="F32" s="9">
+      <c r="F32" s="8">
         <f>3*10^6</f>
         <v>3000000</v>
       </c>
@@ -1011,19 +1149,19 @@
         <f>B35/B39/$B31</f>
         <v>1199.9400029998501</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="8">
         <f>C35/C39/$B31</f>
         <v>470588.23529411765</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="8">
         <f>D35/D39/$B31</f>
         <v>2000000</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E33" s="8">
         <f>E35/E39/$B31</f>
         <v>2666666.6666666665</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F33" s="8">
         <f>F35/F39/$B31</f>
         <v>3000000</v>
       </c>
@@ -1032,23 +1170,23 @@
       <c r="A34" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="2">
         <f>(B33-B32)/B32</f>
         <v>-4.9997500124921622E-5</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="2">
         <f>(C33-C32)/C32</f>
         <v>2.1241830065359485E-2</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="2">
         <f>(D33-D32)/D32</f>
         <v>0</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="2">
         <f>(E33-E32)/E32</f>
         <v>-1.2345679012345737E-2</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="2">
         <f>(F33-F32)/F32</f>
         <v>0</v>
       </c>
@@ -1082,23 +1220,23 @@
       <c r="A36" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="5">
         <f>B35/B32/$B31</f>
         <v>833.33333333333337</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="5">
         <f>C35/C32/$B31</f>
         <v>2.1701388888888888</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="5">
         <f>D35/D32/$B31</f>
         <v>1.5</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="5">
         <f>E35/E32/$B31</f>
         <v>1.1111111111111112</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36" s="5">
         <f>F35/F32/$B31</f>
         <v>1</v>
       </c>
@@ -1107,23 +1245,23 @@
       <c r="A37" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="3">
         <f>FLOOR(B36,1)</f>
         <v>833</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="3">
         <f>FLOOR(C36,1)</f>
         <v>2</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="3">
         <f>FLOOR(D36,1)</f>
         <v>1</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="3">
         <f>FLOOR(E36,1)</f>
         <v>1</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37" s="3">
         <f>FLOOR(F36,1)</f>
         <v>1</v>
       </c>
@@ -1132,23 +1270,23 @@
       <c r="A38" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B38" s="3">
         <f>ROUND((B36-B37)*$B31,0)</f>
         <v>3</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="3">
         <f>ROUND((C36-C37)*$B31,0)</f>
         <v>1</v>
       </c>
-      <c r="D38" s="4">
+      <c r="D38" s="3">
         <f>ROUND((D36-D37)*$B31,0)</f>
         <v>4</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="3">
         <f>ROUND((E36-E37)*$B31,0)</f>
         <v>1</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38" s="3">
         <f>ROUND((F36-F37)*$B31,0)</f>
         <v>0</v>
       </c>
@@ -1157,29 +1295,154 @@
       <c r="A39" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="5">
         <f>B37+B38/$B31</f>
         <v>833.375</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="5">
         <f>C37+C38/$B31</f>
         <v>2.125</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="5">
         <f>D37+D38/$B31</f>
         <v>1.5</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="5">
         <f>E37+E38/$B31</f>
         <v>1.125</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F39" s="5">
         <f>F37+F38/$B31</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E7:E13">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+      <formula>$C7</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>$D7</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2">
+        <v>128</v>
+      </c>
+      <c r="C2" t="str">
+        <f>DEC2HEX(B2)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
output for led driver correct on scope for cmsis
</commit_message>
<xml_diff>
--- a/dwg/LedDriverTiming.xlsx
+++ b/dwg/LedDriverTiming.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -219,47 +219,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -592,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,23 +570,17 @@
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <f>2.6*10^6</f>
-        <v>2600000</v>
-      </c>
-      <c r="C1" s="1">
         <f>2.7*10^6</f>
         <v>2700000</v>
       </c>
-      <c r="D1" s="1">
-        <f>2.4*10^6</f>
-        <v>2400000</v>
-      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
       <c r="H1" t="s">
         <v>25</v>
       </c>
       <c r="I1" s="1">
         <f>9.5*B2</f>
-        <v>3.6538461538461538E-6</v>
+        <v>3.5185185185185183E-6</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -635,14 +589,14 @@
       </c>
       <c r="B2" s="1">
         <f>1/B1</f>
-        <v>3.8461538461538463E-7</v>
+        <v>3.7037037037037036E-7</v>
       </c>
       <c r="H2" t="s">
         <v>27</v>
       </c>
       <c r="I2" s="1">
         <f>I1/3</f>
-        <v>1.217948717948718E-6</v>
+        <v>1.1728395061728394E-6</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -658,7 +612,7 @@
       </c>
       <c r="I3" s="1">
         <f>I2*24</f>
-        <v>2.9230769230769234E-5</v>
+        <v>2.8148148148148143E-5</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -674,7 +628,7 @@
       </c>
       <c r="I4" s="1">
         <f>I3*100+B4</f>
-        <v>2.9730769230769233E-3</v>
+        <v>2.8648148148148144E-3</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -683,7 +637,7 @@
       </c>
       <c r="I5" s="1">
         <f>1/I4</f>
-        <v>336.35187580853813</v>
+        <v>349.06270200387854</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -721,11 +675,11 @@
       </c>
       <c r="E7" s="1">
         <f>1*$B$2</f>
-        <v>3.8461538461538463E-7</v>
+        <v>3.7037037037037036E-7</v>
       </c>
       <c r="G7" s="1">
         <f>E7-C7</f>
-        <v>1.8461538461538466E-7</v>
+        <v>1.703703703703704E-7</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -746,11 +700,11 @@
       </c>
       <c r="E8" s="1">
         <f>2*$B$2</f>
-        <v>7.6923076923076925E-7</v>
+        <v>7.4074074074074073E-7</v>
       </c>
       <c r="G8" s="1">
         <f>E8-C8</f>
-        <v>2.1923076923076933E-7</v>
+        <v>1.907407407407408E-7</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -771,20 +725,11 @@
       </c>
       <c r="E9" s="1">
         <f>2*$B$2</f>
-        <v>7.6923076923076925E-7</v>
+        <v>7.4074074074074073E-7</v>
       </c>
       <c r="G9" s="1">
         <f>E9-C9</f>
-        <v>1.1923076923076934E-7</v>
-      </c>
-      <c r="H9">
-        <v>2.7</v>
-      </c>
-      <c r="I9">
-        <v>2.65</v>
-      </c>
-      <c r="J9">
-        <v>2.6</v>
+        <v>9.0740740740740809E-8</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -805,18 +750,14 @@
       </c>
       <c r="E10" s="9">
         <f>1*$B$2</f>
-        <v>3.8461538461538463E-7</v>
+        <v>3.7037037037037036E-7</v>
       </c>
       <c r="G10" s="1">
         <f>E10-C10</f>
-        <v>-6.53846153846153E-8</v>
-      </c>
-      <c r="H10" s="1">
         <v>-7.9629629629629563E-8</v>
       </c>
-      <c r="I10" s="1">
-        <v>-7.2641509433962205E-8</v>
-      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -837,11 +778,11 @@
       </c>
       <c r="E12" s="1">
         <f>2.5*$B$2</f>
-        <v>9.6153846153846149E-7</v>
+        <v>9.2592592592592594E-7</v>
       </c>
       <c r="G12" s="1">
         <f>E12-C12</f>
-        <v>3.1153846153846157E-7</v>
+        <v>2.7592592592592602E-7</v>
       </c>
       <c r="H12" s="1"/>
     </row>
@@ -863,11 +804,11 @@
       </c>
       <c r="E13" s="1">
         <f>1.5*$B$2</f>
-        <v>5.7692307692307691E-7</v>
+        <v>5.5555555555555552E-7</v>
       </c>
       <c r="G13" s="1">
         <f>E13-C13</f>
-        <v>1.2692307692307699E-7</v>
+        <v>1.0555555555555559E-7</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1318,10 +1259,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E7:E13">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>$C7</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>$D7</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1334,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>